<commit_message>
Redo figures and fix minor issues
</commit_message>
<xml_diff>
--- a/tables/tables.xlsx
+++ b/tables/tables.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\research\_active\CNFL\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25046F65-FB5C-4390-8103-9D9CDB59B77D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA18AB56-5D63-428D-ABB1-60297A869542}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19298" yWindow="-98" windowWidth="19396" windowHeight="10996" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
     <sheet name="Table 2" sheetId="2" r:id="rId2"/>
+    <sheet name="estimates" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
   <si>
     <t>Standard pricing</t>
   </si>
@@ -138,6 +139,42 @@
   </si>
   <si>
     <t>Number of contracts</t>
+  </si>
+  <si>
+    <t>JOINED</t>
+  </si>
+  <si>
+    <t>b=67.89</t>
+  </si>
+  <si>
+    <t>p=0.025</t>
+  </si>
+  <si>
+    <t>JOINED + ALWAYS</t>
+  </si>
+  <si>
+    <t>b=24</t>
+  </si>
+  <si>
+    <t>p=.19</t>
+  </si>
+  <si>
+    <t>LEFT</t>
+  </si>
+  <si>
+    <t>b=16.28</t>
+  </si>
+  <si>
+    <t>p=0.008</t>
+  </si>
+  <si>
+    <t>LEFT +ALWAYS</t>
+  </si>
+  <si>
+    <t>b=6.83</t>
+  </si>
+  <si>
+    <t>p=.209</t>
   </si>
 </sst>
 </file>
@@ -146,7 +183,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -273,38 +310,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -313,14 +323,41 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="5"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -619,13 +656,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="4:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D3" s="1"/>
@@ -635,30 +672,30 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="21"/>
+      <c r="E4" s="29"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="21"/>
+      <c r="H4" s="29"/>
     </row>
     <row r="5" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D5" s="2"/>
       <c r="E5" s="5"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="22"/>
+      <c r="H5" s="30"/>
     </row>
     <row r="6" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="26" t="s">
         <v>21</v>
       </c>
       <c r="F6" s="2"/>
@@ -670,8 +707,8 @@
       </c>
     </row>
     <row r="7" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D7" s="23"/>
-      <c r="E7" s="18"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="26"/>
       <c r="F7" s="2"/>
       <c r="G7" s="3" t="s">
         <v>4</v>
@@ -692,21 +729,21 @@
       </c>
     </row>
     <row r="9" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="26" t="s">
         <v>22</v>
       </c>
       <c r="F9" s="2"/>
-      <c r="G9" s="22" t="s">
+      <c r="G9" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="22"/>
+      <c r="H9" s="30"/>
     </row>
     <row r="10" spans="4:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="23"/>
-      <c r="E10" s="18"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="26"/>
       <c r="F10" s="2"/>
       <c r="G10" s="3" t="s">
         <v>3</v>
@@ -727,10 +764,10 @@
       </c>
     </row>
     <row r="12" spans="4:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="26" t="s">
         <v>23</v>
       </c>
       <c r="F12" s="2"/>
@@ -742,13 +779,13 @@
       </c>
     </row>
     <row r="13" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D13" s="23"/>
-      <c r="E13" s="18"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="26"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="22" t="s">
+      <c r="G13" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="22"/>
+      <c r="H13" s="30"/>
     </row>
     <row r="14" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D14" s="3"/>
@@ -762,10 +799,10 @@
       </c>
     </row>
     <row r="15" spans="4:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="27" t="s">
         <v>24</v>
       </c>
       <c r="F15" s="8"/>
@@ -777,8 +814,8 @@
       </c>
     </row>
     <row r="16" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D16" s="17"/>
-      <c r="E16" s="20"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="28"/>
       <c r="F16" s="11"/>
       <c r="G16" s="12" t="s">
         <v>5</v>
@@ -822,7 +859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DA09302-3D5A-4795-ADF0-539A74E31309}">
   <dimension ref="B3:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="C3:D10"/>
     </sheetView>
   </sheetViews>
@@ -833,76 +870,76 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="24"/>
-      <c r="C3" s="15" t="s">
+      <c r="B3" s="15"/>
+      <c r="C3" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="24"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="15"/>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
-      <c r="E4" s="24"/>
+      <c r="E4" s="15"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="24"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="8"/>
       <c r="D5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="24"/>
+      <c r="E5" s="15"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="24"/>
-      <c r="C6" s="25" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="20">
         <v>436865</v>
       </c>
-      <c r="E6" s="24"/>
+      <c r="E6" s="15"/>
     </row>
     <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="24"/>
-      <c r="C7" s="25" t="s">
+      <c r="B7" s="15"/>
+      <c r="C7" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="21">
         <v>6826</v>
       </c>
-      <c r="E7" s="24"/>
+      <c r="E7" s="15"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="24"/>
-      <c r="C8" s="25" t="s">
+      <c r="B8" s="15"/>
+      <c r="C8" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D8" s="20">
         <v>106</v>
       </c>
-      <c r="E8" s="24"/>
+      <c r="E8" s="15"/>
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="24"/>
-      <c r="C9" s="27" t="s">
+      <c r="B9" s="15"/>
+      <c r="C9" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="31">
+      <c r="D9" s="22">
         <v>555</v>
       </c>
-      <c r="E9" s="24"/>
+      <c r="E9" s="15"/>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="24"/>
-      <c r="C10" s="28" t="s">
+      <c r="B10" s="15"/>
+      <c r="C10" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="26">
+      <c r="D10" s="17">
         <v>444352</v>
       </c>
-      <c r="E10" s="24"/>
+      <c r="E10" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -911,4 +948,67 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{058676BF-A026-47E6-9272-CB2B883096D5}">
+  <dimension ref="B3:F8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>